<commit_message>
doc: Add springbucks-data doc
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -101,9 +101,6 @@
     <t>仿写实战案例</t>
   </si>
   <si>
-    <t>springbucks-data</t>
-  </si>
-  <si>
     <t>版本2</t>
   </si>
   <si>
@@ -478,6 +475,10 @@
     <rPh sb="0" eb="1">
       <t>yi'wan'cheng</t>
     </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>springbucks-data</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -602,12 +603,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -616,6 +611,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -900,7 +901,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -915,129 +916,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10" t="s">
+      <c r="G2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="V2" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="4" t="s">
+      <c r="W2" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="X2" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB2" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="AC2" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC2" s="8" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
@@ -1049,8 +1050,8 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="12" t="s">
-        <v>115</v>
+      <c r="E3" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1086,8 +1087,8 @@
         <v>1</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="12" t="s">
-        <v>115</v>
+      <c r="E4" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="1"/>
@@ -1118,13 +1119,13 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>115</v>
+      <c r="E5" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="1"/>
@@ -1155,13 +1156,13 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>115</v>
+      <c r="E6" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="1"/>
@@ -1197,8 +1198,8 @@
         <v>4</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="12" t="s">
-        <v>115</v>
+      <c r="E7" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="6"/>
@@ -1229,13 +1230,13 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>115</v>
+      <c r="E8" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="9"/>
@@ -1266,13 +1267,13 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>115</v>
+      <c r="E9" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1303,13 +1304,13 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>115</v>
+      <c r="E10" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1340,13 +1341,13 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>115</v>
+      <c r="E11" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1382,8 +1383,8 @@
         <v>9</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="12" t="s">
-        <v>115</v>
+      <c r="E12" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1414,13 +1415,13 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>115</v>
+      <c r="E13" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1451,13 +1452,13 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>115</v>
+      <c r="E14" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1488,13 +1489,13 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>115</v>
+      <c r="E15" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1525,13 +1526,13 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>115</v>
+      <c r="E16" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1562,13 +1563,13 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>115</v>
+      <c r="E17" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1599,13 +1600,13 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>115</v>
+      <c r="E18" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1636,13 +1637,13 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>115</v>
+      <c r="E19" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1678,8 +1679,8 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="12" t="s">
-        <v>115</v>
+      <c r="E20" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1715,8 +1716,8 @@
         <v>18</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="13" t="s">
-        <v>116</v>
+      <c r="E21" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -1747,13 +1748,13 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="14" t="s">
-        <v>117</v>
+      <c r="E22" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="1"/>
@@ -1787,8 +1788,8 @@
       <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>117</v>
+      <c r="E23" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="1"/>
@@ -1822,8 +1823,8 @@
       <c r="D24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="14" t="s">
-        <v>117</v>
+      <c r="E24" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="1"/>
@@ -1857,8 +1858,8 @@
       <c r="D25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="14" t="s">
-        <v>117</v>
+      <c r="E25" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="1"/>
@@ -1889,13 +1890,13 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>116</v>
+      <c r="E26" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="9"/>
@@ -1927,10 +1928,10 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="9"/>
@@ -1963,11 +1964,11 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="12" t="s">
-        <v>115</v>
+      <c r="E28" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1998,13 +1999,13 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>115</v>
+      <c r="E29" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -2036,10 +2037,10 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>115</v>
+        <v>25</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2070,13 +2071,13 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>115</v>
+      <c r="E31" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -2108,10 +2109,10 @@
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>115</v>
+        <v>26</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -2144,11 +2145,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="12" t="s">
-        <v>115</v>
+      <c r="E33" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -2179,13 +2180,13 @@
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E34" s="12" t="s">
-        <v>115</v>
+      <c r="E34" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -2217,10 +2218,10 @@
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>115</v>
+        <v>28</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -2251,13 +2252,13 @@
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="12" t="s">
-        <v>115</v>
+      <c r="E36" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -2289,10 +2290,10 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>115</v>
+        <v>29</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -2325,11 +2326,11 @@
         <v>2.4</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="12" t="s">
-        <v>115</v>
+      <c r="E38" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -2360,13 +2361,13 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E39" s="12" t="s">
-        <v>115</v>
+      <c r="E39" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -2398,10 +2399,10 @@
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>115</v>
+        <v>31</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -2432,13 +2433,13 @@
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E41" s="12" t="s">
-        <v>115</v>
+      <c r="E41" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -2470,10 +2471,10 @@
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>115</v>
+        <v>32</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -2506,11 +2507,11 @@
         <v>2.5</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D43" s="1"/>
-      <c r="E43" s="12" t="s">
-        <v>115</v>
+      <c r="E43" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -2541,13 +2542,13 @@
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="12" t="s">
-        <v>115</v>
+      <c r="E44" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -2579,10 +2580,10 @@
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>115</v>
+        <v>34</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -2613,13 +2614,13 @@
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E46" s="12" t="s">
-        <v>115</v>
+      <c r="E46" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -2651,10 +2652,10 @@
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>115</v>
+        <v>35</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -2687,11 +2688,11 @@
         <v>2.6</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D48" s="1"/>
-      <c r="E48" s="12" t="s">
-        <v>115</v>
+      <c r="E48" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -2722,13 +2723,13 @@
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E49" s="12" t="s">
-        <v>115</v>
+      <c r="E49" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2760,10 +2761,10 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>115</v>
+        <v>37</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -2794,13 +2795,13 @@
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E51" s="12" t="s">
-        <v>115</v>
+      <c r="E51" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -2832,10 +2833,10 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>115</v>
+        <v>38</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -2868,11 +2869,11 @@
         <v>2.7</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D53" s="1"/>
-      <c r="E53" s="12" t="s">
-        <v>115</v>
+      <c r="E53" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -2903,13 +2904,13 @@
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E54" s="12" t="s">
-        <v>115</v>
+      <c r="E54" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -2941,10 +2942,10 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>115</v>
+        <v>40</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -2976,10 +2977,10 @@
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>115</v>
+        <v>41</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -3010,13 +3011,13 @@
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E57" s="12" t="s">
-        <v>115</v>
+      <c r="E57" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -3048,10 +3049,10 @@
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>115</v>
+        <v>42</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -3084,11 +3085,11 @@
         <v>2.8</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D59" s="1"/>
-      <c r="E59" s="12" t="s">
-        <v>115</v>
+      <c r="E59" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -3119,13 +3120,13 @@
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E60" s="12" t="s">
-        <v>115</v>
+      <c r="E60" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -3157,10 +3158,10 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>115</v>
+        <v>108</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -3192,10 +3193,10 @@
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>115</v>
+        <v>44</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -3226,13 +3227,13 @@
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E63" s="12" t="s">
-        <v>115</v>
+      <c r="E63" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -3264,10 +3265,10 @@
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>115</v>
+        <v>45</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -3300,11 +3301,11 @@
         <v>2.9</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D65" s="1"/>
-      <c r="E65" s="12" t="s">
-        <v>115</v>
+      <c r="E65" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -3335,13 +3336,13 @@
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E66" s="12" t="s">
-        <v>115</v>
+      <c r="E66" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -3373,10 +3374,10 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E67" s="12" t="s">
-        <v>115</v>
+        <v>47</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -3407,13 +3408,13 @@
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E68" s="12" t="s">
-        <v>115</v>
+      <c r="E68" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -3445,10 +3446,10 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>115</v>
+        <v>48</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -3478,14 +3479,14 @@
     <row r="70" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D70" s="1"/>
-      <c r="E70" s="12" t="s">
-        <v>115</v>
+      <c r="E70" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -3516,13 +3517,13 @@
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E71" s="12" t="s">
-        <v>115</v>
+      <c r="E71" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -3554,10 +3555,10 @@
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E72" s="12" t="s">
-        <v>115</v>
+        <v>50</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -3588,13 +3589,13 @@
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E73" s="12" t="s">
-        <v>115</v>
+      <c r="E73" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -3626,10 +3627,10 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>115</v>
+        <v>51</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -3662,11 +3663,11 @@
         <v>2.11</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D75" s="1"/>
-      <c r="E75" s="12" t="s">
-        <v>115</v>
+      <c r="E75" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
@@ -3697,13 +3698,13 @@
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E76" s="12" t="s">
-        <v>115</v>
+      <c r="E76" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -3735,10 +3736,10 @@
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E77" s="12" t="s">
-        <v>115</v>
+        <v>53</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -3769,13 +3770,13 @@
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E78" s="12" t="s">
-        <v>115</v>
+      <c r="E78" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -3807,10 +3808,10 @@
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>115</v>
+        <v>54</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -3843,11 +3844,11 @@
         <v>2.12</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D80" s="1"/>
-      <c r="E80" s="12" t="s">
-        <v>115</v>
+      <c r="E80" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -3878,13 +3879,13 @@
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E81" s="12" t="s">
-        <v>115</v>
+      <c r="E81" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -3916,10 +3917,10 @@
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E82" s="12" t="s">
-        <v>115</v>
+        <v>56</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
@@ -3950,13 +3951,13 @@
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E83" s="12" t="s">
-        <v>115</v>
+      <c r="E83" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
@@ -3988,10 +3989,10 @@
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E84" s="12" t="s">
-        <v>115</v>
+        <v>57</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>

</xml_diff>

<commit_message>
feat: Add demo for reactor basic
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -613,15 +613,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -902,10 +902,10 @@
   <dimension ref="A1:AC84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H39" sqref="H39"/>
+      <selection pane="bottomRight" activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -920,58 +920,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12" t="s">
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12" t="s">
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12" t="s">
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12" t="s">
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12" t="s">
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="4" t="s">
         <v>98</v>
       </c>
@@ -1057,8 +1057,8 @@
       <c r="E3" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -1686,8 +1686,8 @@
       <c r="E20" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -1723,8 +1723,8 @@
       <c r="E21" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
       <c r="H21" s="7"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1760,7 +1760,7 @@
       <c r="E22" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="F22" s="16"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1795,7 +1795,7 @@
       <c r="E23" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="F23" s="16"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1830,7 +1830,7 @@
       <c r="E24" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="F24" s="16"/>
+      <c r="F24" s="14"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1865,7 +1865,7 @@
       <c r="E25" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="F25" s="16"/>
+      <c r="F25" s="14"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1903,7 +1903,7 @@
         <v>115</v>
       </c>
       <c r="F26" s="1"/>
-      <c r="G26" s="16"/>
+      <c r="G26" s="14"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1938,7 +1938,7 @@
         <v>115</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="16"/>
+      <c r="G27" s="14"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1976,8 +1976,8 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="9"/>
+      <c r="H29" s="14"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -2048,7 +2048,7 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="9"/>
+      <c r="H30" s="14"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -2086,7 +2086,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="9"/>
+      <c r="I31" s="14"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -2121,7 +2121,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="9"/>
+      <c r="I32" s="14"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>

</xml_diff>

<commit_message>
feat: Add demo for reactive redis
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="28020" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="480" windowWidth="28020" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -901,11 +901,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J33" sqref="J33"/>
+      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1971,8 +1971,8 @@
         <v>24</v>
       </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="10" t="s">
-        <v>114</v>
+      <c r="E28" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -2008,8 +2008,8 @@
       <c r="D29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>114</v>
+      <c r="E29" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -2043,8 +2043,8 @@
       <c r="D30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>114</v>
+      <c r="E30" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2080,8 +2080,8 @@
       <c r="D31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="10" t="s">
-        <v>114</v>
+      <c r="E31" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -2115,8 +2115,8 @@
       <c r="D32" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>114</v>
+      <c r="E32" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>

</xml_diff>